<commit_message>
Added information about additional CMIP6 computer
</commit_message>
<xml_diff>
--- a/cmip6/machines/cmip6_ncc_machines.xlsx
+++ b/cmip6/machines/cmip6_ncc_machines.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="321">
   <si>
     <t xml:space="preserve">ES-DOC CMIP6 Institute Machines</t>
   </si>
@@ -1028,6 +1028,47 @@
   <si>
     <t xml:space="preserve">all</t>
   </si>
+  <si>
+    <t xml:space="preserve">Vilje</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vilje is a cluster system procured by NTNU, in cooperation with the Norwegian
+Meteorological Institute and UNINETT Sigma in 2012. Vilje is used for numerical
+weather prediction in operational forecasting by met.no, as well as for research
+in a broad range of topics at NTNU and other Norwegian universities, colleges
+and research institutes.
+Vilje is a distributed memory system that consists of 1440 nodes interconnected
+with a high-bandwidth low-latency switch network (FDR Infiniband). Each node has
+two 8-core Intel Sandy Bridge (2.6 Ghz) and 32 GB memory. The total number of
+cores is 23040.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.sigma2.no/systems#vilje</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SGI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Altix 8600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vilje is a distributed memory system that consists of 1440 nodes interconnected
+with a high-bandwidth low-latency switch network (FDR Infiniband). Each node has
+two 8-core Intel Sandy Bridge (2.6 Ghz) and 32 GB memory. The total number of
+cores is 23040.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32 GiB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intel Sandy Bridge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some</t>
+  </si>
 </sst>
 </file>
 
@@ -1038,7 +1079,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
-  <fonts count="33">
+  <fonts count="34">
     <font>
       <sz val="10"/>
       <name val="Helvetica Neue"/>
@@ -1265,6 +1306,11 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -1385,7 +1431,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1644,6 +1690,10 @@
     </xf>
     <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -6771,7 +6821,7 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A365" colorId="64" zoomScale="69" zoomScaleNormal="69" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A365" colorId="64" zoomScale="69" zoomScaleNormal="69" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A422" activeCellId="0" sqref="A422"/>
     </sheetView>
   </sheetViews>
@@ -11642,8 +11692,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="69" zoomScaleNormal="69" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A463" colorId="64" zoomScale="69" zoomScaleNormal="69" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B470" activeCellId="0" sqref="B470"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11762,7 +11812,9 @@
     </row>
     <row r="11" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0"/>
-      <c r="B11" s="26"/>
+      <c r="B11" s="26" t="s">
+        <v>311</v>
+      </c>
       <c r="C11" s="26"/>
       <c r="D11" s="26"/>
       <c r="E11" s="0"/>
@@ -11918,7 +11970,9 @@
     </row>
     <row r="27" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="30"/>
-      <c r="B27" s="31"/>
+      <c r="B27" s="31" t="s">
+        <v>297</v>
+      </c>
       <c r="C27" s="31"/>
       <c r="D27" s="31"/>
       <c r="E27" s="0"/>
@@ -11958,7 +12012,9 @@
     </row>
     <row r="31" customFormat="false" ht="148.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0"/>
-      <c r="B31" s="31"/>
+      <c r="B31" s="31" t="s">
+        <v>312</v>
+      </c>
       <c r="C31" s="31"/>
       <c r="D31" s="31"/>
       <c r="E31" s="0"/>
@@ -12016,7 +12072,9 @@
     </row>
     <row r="37" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0"/>
-      <c r="B37" s="26"/>
+      <c r="B37" s="26" t="s">
+        <v>313</v>
+      </c>
       <c r="C37" s="26"/>
       <c r="D37" s="26"/>
       <c r="E37" s="0"/>
@@ -12076,7 +12134,9 @@
       <c r="A43" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="B43" s="31"/>
+      <c r="B43" s="31" t="n">
+        <v>2012</v>
+      </c>
       <c r="C43" s="31"/>
       <c r="D43" s="31"/>
       <c r="E43" s="0"/>
@@ -12094,7 +12154,9 @@
       <c r="A45" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="B45" s="31"/>
+      <c r="B45" s="31" t="s">
+        <v>314</v>
+      </c>
       <c r="C45" s="31"/>
       <c r="D45" s="31"/>
       <c r="E45" s="0"/>
@@ -12134,7 +12196,9 @@
     </row>
     <row r="49" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="0"/>
-      <c r="B49" s="26"/>
+      <c r="B49" s="26" t="s">
+        <v>300</v>
+      </c>
       <c r="C49" s="26"/>
       <c r="D49" s="26"/>
       <c r="E49" s="0"/>
@@ -12222,7 +12286,9 @@
     </row>
     <row r="58" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="0"/>
-      <c r="B58" s="26"/>
+      <c r="B58" s="26" t="s">
+        <v>315</v>
+      </c>
       <c r="C58" s="26"/>
       <c r="D58" s="26"/>
       <c r="E58" s="0"/>
@@ -12262,7 +12328,9 @@
     </row>
     <row r="62" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="0"/>
-      <c r="B62" s="26"/>
+      <c r="B62" s="26" t="s">
+        <v>316</v>
+      </c>
       <c r="C62" s="26"/>
       <c r="D62" s="26"/>
       <c r="E62" s="0"/>
@@ -12420,9 +12488,11 @@
     </row>
     <row r="78" customFormat="false" ht="221.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="0"/>
-      <c r="B78" s="31"/>
-      <c r="C78" s="31"/>
-      <c r="D78" s="31"/>
+      <c r="B78" s="65" t="s">
+        <v>317</v>
+      </c>
+      <c r="C78" s="65"/>
+      <c r="D78" s="65"/>
       <c r="E78" s="0"/>
       <c r="F78" s="0"/>
     </row>
@@ -12558,7 +12628,9 @@
     </row>
     <row r="92" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="0"/>
-      <c r="B92" s="26"/>
+      <c r="B92" s="26" t="n">
+        <v>1440</v>
+      </c>
       <c r="C92" s="26"/>
       <c r="D92" s="26"/>
       <c r="E92" s="0"/>
@@ -12598,7 +12670,9 @@
     </row>
     <row r="96" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="0"/>
-      <c r="B96" s="26"/>
+      <c r="B96" s="26" t="s">
+        <v>318</v>
+      </c>
       <c r="C96" s="26"/>
       <c r="D96" s="26"/>
       <c r="E96" s="0"/>
@@ -12638,7 +12712,9 @@
     </row>
     <row r="100" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="0"/>
-      <c r="B100" s="26"/>
+      <c r="B100" s="26" t="n">
+        <v>16</v>
+      </c>
       <c r="C100" s="26"/>
       <c r="D100" s="26"/>
       <c r="E100" s="0"/>
@@ -13262,7 +13338,9 @@
     </row>
     <row r="162" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A162" s="0"/>
-      <c r="B162" s="51"/>
+      <c r="B162" s="51" t="s">
+        <v>319</v>
+      </c>
       <c r="C162" s="0"/>
       <c r="D162" s="0"/>
       <c r="E162" s="0"/>
@@ -13302,7 +13380,9 @@
     </row>
     <row r="166" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="0"/>
-      <c r="B166" s="51"/>
+      <c r="B166" s="51" t="n">
+        <v>2.6</v>
+      </c>
       <c r="C166" s="0"/>
       <c r="D166" s="0"/>
       <c r="E166" s="0"/>
@@ -13342,7 +13422,9 @@
     </row>
     <row r="170" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A170" s="0"/>
-      <c r="B170" s="51"/>
+      <c r="B170" s="51" t="n">
+        <v>2</v>
+      </c>
       <c r="C170" s="0"/>
       <c r="D170" s="0"/>
       <c r="E170" s="0"/>
@@ -15312,7 +15394,9 @@
     </row>
     <row r="381" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A381" s="30"/>
-      <c r="B381" s="31"/>
+      <c r="B381" s="31" t="s">
+        <v>320</v>
+      </c>
       <c r="C381" s="31"/>
       <c r="D381" s="31"/>
     </row>
@@ -15568,7 +15652,9 @@
     </row>
     <row r="413" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A413" s="30"/>
-      <c r="B413" s="31"/>
+      <c r="B413" s="31" t="s">
+        <v>225</v>
+      </c>
       <c r="C413" s="31"/>
       <c r="D413" s="31"/>
     </row>
@@ -15998,11 +16084,13 @@
       <c r="C467" s="23"/>
       <c r="D467" s="23"/>
     </row>
-    <row r="468" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="468" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A468" s="28" t="s">
         <v>178</v>
       </c>
-      <c r="B468" s="31"/>
+      <c r="B468" s="31" t="s">
+        <v>309</v>
+      </c>
       <c r="C468" s="31"/>
       <c r="D468" s="31"/>
     </row>
@@ -16459,6 +16547,9 @@
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B37" r:id="rId1" location="vilje" display="https://www.sigma2.no/systems#vilje"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.277777777777778"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>